<commit_message>
TODOS LOS TESTS FUNCIONANDOOO
</commit_message>
<xml_diff>
--- a/Grupo_L-tests/Datos alumnadoFAKE.xlsx
+++ b/Grupo_L-tests/Datos alumnadoFAKE.xlsx
@@ -503,7 +503,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,7 +580,7 @@
   <dimension ref="A1:AA1513"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>